<commit_message>
Integracion de BD y descarga de información proveniente de la BD
</commit_message>
<xml_diff>
--- a/modulo/MOCK_DATA.xlsx
+++ b/modulo/MOCK_DATA.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Desktop\Disagro\Proyecto_I_Analisis_y_Diseno\modulo\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62472AAA-5105-4993-B32D-924073AC535F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="564" windowWidth="10272" windowHeight="12396" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="data"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -1228,12 +1222,21 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <name val="Arial"/>
-      <family val="1"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1244,7 +1247,14 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -1256,34 +1266,46 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="6">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -1310,116 +1332,82 @@
         <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="467886"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607D"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1431,2204 +1419,2207 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:tint val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:tint val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="9500"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot rev="0" lon="0" lat="0"/>
+            </a:camera>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:tint val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="B70" workbookViewId="0">
-      <selection activeCell="D77" sqref="D77"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.69921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.09765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="4" width="6.433571428571429" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="9.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="5" width="24.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="4" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="5" width="33.86214285714286" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="3">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="3">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="3">
         <v>3</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="3">
         <v>4</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="3">
         <v>5</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="3">
         <v>6</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="3">
         <v>7</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="3">
         <v>8</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="3">
         <v>9</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="3">
         <v>10</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+      <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="3">
         <v>11</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+      <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="3">
         <v>12</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+      <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="3">
         <v>13</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+      <c r="A15" s="3">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="3">
         <v>14</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+      <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="3">
         <v>15</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+      <c r="A17" s="3">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="3">
         <v>16</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+      <c r="A18" s="3">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="3">
         <v>17</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+      <c r="A19" s="3">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="3">
         <v>18</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+      <c r="A20" s="3">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="3">
         <v>19</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+      <c r="A21" s="3">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="3">
         <v>20</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+      <c r="A22" s="3">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="3">
         <v>21</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+      <c r="A23" s="3">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="3">
         <v>22</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+      <c r="A24" s="3">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="3">
         <v>23</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+      <c r="A25" s="3">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="3">
         <v>24</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+      <c r="A26" s="3">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="3">
         <v>25</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+      <c r="A27" s="3">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="3">
         <v>26</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+      <c r="A28" s="3">
         <v>27</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="3">
         <v>27</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+      <c r="A29" s="3">
         <v>28</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="3">
         <v>28</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+      <c r="A30" s="3">
         <v>29</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="3">
         <v>29</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+      <c r="A31" s="3">
         <v>30</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="3">
         <v>30</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
+      <c r="A32" s="3">
         <v>31</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="3">
         <v>31</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
+      <c r="A33" s="3">
         <v>32</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="3">
         <v>32</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F33" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
+      <c r="A34" s="3">
         <v>33</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="3">
         <v>33</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F34" s="2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
+      <c r="A35" s="3">
         <v>34</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="3">
         <v>34</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F35" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
+      <c r="A36" s="3">
         <v>35</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="3">
         <v>35</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F36" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
+      <c r="A37" s="3">
         <v>36</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="3">
         <v>36</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F37" s="2" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
+      <c r="A38" s="3">
         <v>37</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="3">
         <v>37</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F38" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
+      <c r="A39" s="3">
         <v>38</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="3">
         <v>38</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F39" s="2" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
+      <c r="A40" s="3">
         <v>39</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="3">
         <v>39</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F40" s="2" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
+      <c r="A41" s="3">
         <v>40</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="3">
         <v>40</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F41" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42">
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
+      <c r="A42" s="3">
         <v>41</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="3">
         <v>41</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F42" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43">
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
+      <c r="A43" s="3">
         <v>42</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="E43">
+      <c r="E43" s="3">
         <v>42</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F43" s="2" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44">
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
+      <c r="A44" s="3">
         <v>43</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="E44">
+      <c r="E44" s="3">
         <v>43</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F44" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45">
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
+      <c r="A45" s="3">
         <v>44</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="3">
         <v>44</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F45" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46">
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
+      <c r="A46" s="3">
         <v>45</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="E46">
+      <c r="E46" s="3">
         <v>45</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F46" s="2" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47">
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
+      <c r="A47" s="3">
         <v>46</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="E47">
+      <c r="E47" s="3">
         <v>46</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F47" s="2" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48">
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
+      <c r="A48" s="3">
         <v>47</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="E48">
+      <c r="E48" s="3">
         <v>47</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F48" s="2" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49">
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
+      <c r="A49" s="3">
         <v>48</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="E49">
+      <c r="E49" s="3">
         <v>48</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F49" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50">
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
+      <c r="A50" s="3">
         <v>49</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="E50">
+      <c r="E50" s="3">
         <v>49</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F50" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51">
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
+      <c r="A51" s="3">
         <v>50</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="E51">
+      <c r="E51" s="3">
         <v>50</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F51" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52">
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
+      <c r="A52" s="3">
         <v>51</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="E52">
+      <c r="E52" s="3">
         <v>51</v>
       </c>
-      <c r="F52" t="s">
+      <c r="F52" s="2" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53">
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
+      <c r="A53" s="3">
         <v>52</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D53" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="E53">
+      <c r="E53" s="3">
         <v>52</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F53" s="2" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54">
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
+      <c r="A54" s="3">
         <v>53</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D54" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="E54">
+      <c r="E54" s="3">
         <v>53</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F54" s="2" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55">
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
+      <c r="A55" s="3">
         <v>54</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D55" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="E55">
+      <c r="E55" s="3">
         <v>54</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F55" s="2" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56">
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
+      <c r="A56" s="3">
         <v>55</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D56" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="E56">
+      <c r="E56" s="3">
         <v>55</v>
       </c>
-      <c r="F56" t="s">
+      <c r="F56" s="2" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57">
+    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
+      <c r="A57" s="3">
         <v>56</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D57" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="E57">
+      <c r="E57" s="3">
         <v>56</v>
       </c>
-      <c r="F57" t="s">
+      <c r="F57" s="2" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58">
+    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
+      <c r="A58" s="3">
         <v>57</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D58" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="E58">
+      <c r="E58" s="3">
         <v>57</v>
       </c>
-      <c r="F58" t="s">
+      <c r="F58" s="2" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59">
+    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
+      <c r="A59" s="3">
         <v>58</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D59" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="E59">
+      <c r="E59" s="3">
         <v>58</v>
       </c>
-      <c r="F59" t="s">
+      <c r="F59" s="2" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60">
+    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
+      <c r="A60" s="3">
         <v>59</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D60" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="E60">
+      <c r="E60" s="3">
         <v>59</v>
       </c>
-      <c r="F60" t="s">
+      <c r="F60" s="2" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61">
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
+      <c r="A61" s="3">
         <v>60</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D61" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="E61">
+      <c r="E61" s="3">
         <v>60</v>
       </c>
-      <c r="F61" t="s">
+      <c r="F61" s="2" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62">
+    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
+      <c r="A62" s="3">
         <v>61</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D62" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="E62">
+      <c r="E62" s="3">
         <v>61</v>
       </c>
-      <c r="F62" t="s">
+      <c r="F62" s="2" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63">
+    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
+      <c r="A63" s="3">
         <v>62</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D63" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E63">
+      <c r="E63" s="3">
         <v>62</v>
       </c>
-      <c r="F63" t="s">
+      <c r="F63" s="2" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64">
+    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
+      <c r="A64" s="3">
         <v>63</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D64" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="E64">
+      <c r="E64" s="3">
         <v>63</v>
       </c>
-      <c r="F64" t="s">
+      <c r="F64" s="2" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65">
+    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
+      <c r="A65" s="3">
         <v>64</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D65" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="E65">
+      <c r="E65" s="3">
         <v>64</v>
       </c>
-      <c r="F65" t="s">
+      <c r="F65" s="2" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66">
+    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
+      <c r="A66" s="3">
         <v>65</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D66" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="E66">
+      <c r="E66" s="3">
         <v>65</v>
       </c>
-      <c r="F66" t="s">
+      <c r="F66" s="2" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67">
+    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
+      <c r="A67" s="3">
         <v>66</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D67" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="E67">
+      <c r="E67" s="3">
         <v>66</v>
       </c>
-      <c r="F67" t="s">
+      <c r="F67" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68">
+    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
+      <c r="A68" s="3">
         <v>67</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="D68" t="s">
+      <c r="D68" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="E68">
+      <c r="E68" s="3">
         <v>67</v>
       </c>
-      <c r="F68" t="s">
+      <c r="F68" s="2" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69">
+    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
+      <c r="A69" s="3">
         <v>68</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D69" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="E69">
+      <c r="E69" s="3">
         <v>68</v>
       </c>
-      <c r="F69" t="s">
+      <c r="F69" s="2" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70">
+    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
+      <c r="A70" s="3">
         <v>69</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C70" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D70" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="E70">
+      <c r="E70" s="3">
         <v>69</v>
       </c>
-      <c r="F70" t="s">
+      <c r="F70" s="2" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71">
+    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
+      <c r="A71" s="3">
         <v>70</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D71" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="E71">
+      <c r="E71" s="3">
         <v>70</v>
       </c>
-      <c r="F71" t="s">
+      <c r="F71" s="2" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72">
+    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
+      <c r="A72" s="3">
         <v>71</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C72" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D72" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="E72">
+      <c r="E72" s="3">
         <v>71</v>
       </c>
-      <c r="F72" t="s">
+      <c r="F72" s="2" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73">
+    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
+      <c r="A73" s="3">
         <v>72</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C73" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D73" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="E73">
+      <c r="E73" s="3">
         <v>72</v>
       </c>
-      <c r="F73" t="s">
+      <c r="F73" s="2" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74">
+    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
+      <c r="A74" s="3">
         <v>73</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="D74" t="s">
+      <c r="D74" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="E74">
+      <c r="E74" s="3">
         <v>73</v>
       </c>
-      <c r="F74" t="s">
+      <c r="F74" s="2" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75">
+    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75">
+      <c r="A75" s="3">
         <v>74</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D75" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="E75">
+      <c r="E75" s="3">
         <v>74</v>
       </c>
-      <c r="F75" t="s">
+      <c r="F75" s="2" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76">
+    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
+      <c r="A76" s="3">
         <v>75</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="D76" t="s">
+      <c r="D76" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="E76">
+      <c r="E76" s="3">
         <v>75</v>
       </c>
-      <c r="F76" t="s">
+      <c r="F76" s="2" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77">
+    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
+      <c r="A77" s="3">
         <v>76</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C77" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D77" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="E77">
+      <c r="E77" s="3">
         <v>76</v>
       </c>
-      <c r="F77" t="s">
+      <c r="F77" s="2" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78">
+    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
+      <c r="A78" s="3">
         <v>77</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C78" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D78" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="E78">
+      <c r="E78" s="3">
         <v>77</v>
       </c>
-      <c r="F78" t="s">
+      <c r="F78" s="2" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79">
+    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
+      <c r="A79" s="3">
         <v>78</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B79" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C79" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="D79" t="s">
+      <c r="D79" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="E79">
+      <c r="E79" s="3">
         <v>78</v>
       </c>
-      <c r="F79" t="s">
+      <c r="F79" s="2" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80">
+    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
+      <c r="A80" s="3">
         <v>79</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C80" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="D80" t="s">
+      <c r="D80" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="E80">
+      <c r="E80" s="3">
         <v>79</v>
       </c>
-      <c r="F80" t="s">
+      <c r="F80" s="2" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81">
+    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
+      <c r="A81" s="3">
         <v>80</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B81" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C81" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="D81" t="s">
+      <c r="D81" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="E81">
+      <c r="E81" s="3">
         <v>80</v>
       </c>
-      <c r="F81" t="s">
+      <c r="F81" s="2" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82">
+    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75">
+      <c r="A82" s="3">
         <v>81</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C82" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="D82" t="s">
+      <c r="D82" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="E82">
+      <c r="E82" s="3">
         <v>81</v>
       </c>
-      <c r="F82" t="s">
+      <c r="F82" s="2" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83">
+    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75">
+      <c r="A83" s="3">
         <v>82</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B83" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C83" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="D83" t="s">
+      <c r="D83" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="E83">
+      <c r="E83" s="3">
         <v>82</v>
       </c>
-      <c r="F83" t="s">
+      <c r="F83" s="2" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84">
+    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75">
+      <c r="A84" s="3">
         <v>83</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C84" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="D84" t="s">
+      <c r="D84" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="E84">
+      <c r="E84" s="3">
         <v>83</v>
       </c>
-      <c r="F84" t="s">
+      <c r="F84" s="2" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85">
+    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
+      <c r="A85" s="3">
         <v>84</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B85" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C85" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D85" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="E85">
+      <c r="E85" s="3">
         <v>84</v>
       </c>
-      <c r="F85" t="s">
+      <c r="F85" s="2" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86">
+    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
+      <c r="A86" s="3">
         <v>85</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B86" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C86" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D86" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="E86">
+      <c r="E86" s="3">
         <v>85</v>
       </c>
-      <c r="F86" t="s">
+      <c r="F86" s="2" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87">
+    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
+      <c r="A87" s="3">
         <v>86</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B87" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C87" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D87" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="E87">
+      <c r="E87" s="3">
         <v>86</v>
       </c>
-      <c r="F87" t="s">
+      <c r="F87" s="2" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88">
+    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
+      <c r="A88" s="3">
         <v>87</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B88" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C88" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="D88" t="s">
+      <c r="D88" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="E88">
+      <c r="E88" s="3">
         <v>87</v>
       </c>
-      <c r="F88" t="s">
+      <c r="F88" s="2" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89">
+    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
+      <c r="A89" s="3">
         <v>88</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B89" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C89" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="D89" t="s">
+      <c r="D89" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="E89">
+      <c r="E89" s="3">
         <v>88</v>
       </c>
-      <c r="F89" t="s">
+      <c r="F89" s="2" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90">
+    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
+      <c r="A90" s="3">
         <v>89</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B90" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C90" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="D90" t="s">
+      <c r="D90" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="E90">
+      <c r="E90" s="3">
         <v>89</v>
       </c>
-      <c r="F90" t="s">
+      <c r="F90" s="2" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91">
+    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
+      <c r="A91" s="3">
         <v>90</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B91" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C91" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="D91" t="s">
+      <c r="D91" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="E91">
+      <c r="E91" s="3">
         <v>90</v>
       </c>
-      <c r="F91" t="s">
+      <c r="F91" s="2" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92">
+    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
+      <c r="A92" s="3">
         <v>91</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B92" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C92" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="D92" t="s">
+      <c r="D92" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="E92">
+      <c r="E92" s="3">
         <v>91</v>
       </c>
-      <c r="F92" t="s">
+      <c r="F92" s="2" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93">
+    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
+      <c r="A93" s="3">
         <v>92</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B93" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C93" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="D93" t="s">
+      <c r="D93" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="E93">
+      <c r="E93" s="3">
         <v>92</v>
       </c>
-      <c r="F93" t="s">
+      <c r="F93" s="2" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94">
+    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75">
+      <c r="A94" s="3">
         <v>93</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B94" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C94" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D94" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="E94">
+      <c r="E94" s="3">
         <v>93</v>
       </c>
-      <c r="F94" t="s">
+      <c r="F94" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95">
+    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75">
+      <c r="A95" s="3">
         <v>94</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B95" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C95" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="D95" t="s">
+      <c r="D95" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="E95">
+      <c r="E95" s="3">
         <v>94</v>
       </c>
-      <c r="F95" t="s">
+      <c r="F95" s="2" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96">
+    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
+      <c r="A96" s="3">
         <v>95</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B96" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C96" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D96" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="E96">
+      <c r="E96" s="3">
         <v>95</v>
       </c>
-      <c r="F96" t="s">
+      <c r="F96" s="2" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97">
+    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
+      <c r="A97" s="3">
         <v>96</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B97" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C97" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="D97" t="s">
+      <c r="D97" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="E97">
+      <c r="E97" s="3">
         <v>96</v>
       </c>
-      <c r="F97" t="s">
+      <c r="F97" s="2" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98">
+    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75">
+      <c r="A98" s="3">
         <v>97</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B98" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C98" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="D98" t="s">
+      <c r="D98" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="E98">
+      <c r="E98" s="3">
         <v>97</v>
       </c>
-      <c r="F98" t="s">
+      <c r="F98" s="2" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99">
+    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75">
+      <c r="A99" s="3">
         <v>98</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B99" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C99" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D99" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="E99">
+      <c r="E99" s="3">
         <v>98</v>
       </c>
-      <c r="F99" t="s">
+      <c r="F99" s="2" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100">
+    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18.75">
+      <c r="A100" s="3">
         <v>99</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B100" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C100" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="D100" t="s">
+      <c r="D100" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="E100">
+      <c r="E100" s="3">
         <v>99</v>
       </c>
-      <c r="F100" t="s">
+      <c r="F100" s="2" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101">
+    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="18.75">
+      <c r="A101" s="3">
         <v>100</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B101" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C101" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="D101" t="s">
+      <c r="D101" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="E101">
+      <c r="E101" s="3">
         <v>100</v>
       </c>
-      <c r="F101" t="s">
+      <c r="F101" s="2" t="s">
         <v>327</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>